<commit_message>
update course content for spark and scala
</commit_message>
<xml_diff>
--- a/AgileWork/Hadoop_Scala_Spark.xlsx
+++ b/AgileWork/Hadoop_Scala_Spark.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="13760" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="13760" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Apache Hadoop" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="MISCILLANEOUS" sheetId="5" r:id="rId6"/>
     <sheet name="SCALA" sheetId="6" r:id="rId7"/>
     <sheet name="APACHE SPARK" sheetId="7" r:id="rId8"/>
+    <sheet name="OthersUseful" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="289">
   <si>
     <t>Day</t>
   </si>
@@ -324,9 +325,6 @@
     <t>Package Object</t>
   </si>
   <si>
-    <t>TODO</t>
-  </si>
-  <si>
     <t>GENERICS</t>
   </si>
   <si>
@@ -360,24 +358,15 @@
     <t>Saprk Architecture and SparkContext</t>
   </si>
   <si>
-    <t>Spark Modes</t>
-  </si>
-  <si>
     <t>Spark on Shell</t>
   </si>
   <si>
     <t>Spark web UI</t>
   </si>
   <si>
-    <t>What is RDD</t>
-  </si>
-  <si>
     <t>Features of RDD's</t>
   </si>
   <si>
-    <t>RDD workflow</t>
-  </si>
-  <si>
     <t>RDD Transformations and Actions</t>
   </si>
   <si>
@@ -423,30 +412,9 @@
     <t>What is streaming</t>
   </si>
   <si>
-    <t>Spark Ecosystem</t>
-  </si>
-  <si>
-    <t>Spark Streaming Works</t>
-  </si>
-  <si>
-    <t>Spark Streaming Workflow</t>
-  </si>
-  <si>
-    <t>Spark Streaming Fundamentals</t>
-  </si>
-  <si>
-    <t>Streaming Context</t>
-  </si>
-  <si>
-    <t>Dstreams</t>
-  </si>
-  <si>
     <t>Spark SQL</t>
   </si>
   <si>
-    <t>Why Spark SQL</t>
-  </si>
-  <si>
     <t>What is Spark SQL</t>
   </si>
   <si>
@@ -840,9 +808,6 @@
     <t>SPARK CORE</t>
   </si>
   <si>
-    <t>Key Value RDD</t>
-  </si>
-  <si>
     <t xml:space="preserve">Data Partitioning </t>
   </si>
   <si>
@@ -877,6 +842,66 @@
   </si>
   <si>
     <t>BroadCast Variable</t>
+  </si>
+  <si>
+    <t>Some</t>
+  </si>
+  <si>
+    <t>hadoop fs -ls -count -q /user/edureka</t>
+  </si>
+  <si>
+    <t>Spark deployement Modes</t>
+  </si>
+  <si>
+    <t>Spark Clusters</t>
+  </si>
+  <si>
+    <t>What is RDD ?</t>
+  </si>
+  <si>
+    <t>CREATING RDD</t>
+  </si>
+  <si>
+    <t>Common Transformations and Actions</t>
+  </si>
+  <si>
+    <t>Key Value Pair RDD</t>
+  </si>
+  <si>
+    <t>Creating Pair RDD</t>
+  </si>
+  <si>
+    <t>RDD Lineage Graph</t>
+  </si>
+  <si>
+    <t>Helloworld With SBT</t>
+  </si>
+  <si>
+    <t>Creating Spark Helloworld Program in scala</t>
+  </si>
+  <si>
+    <t>Executing through spark-submit</t>
+  </si>
+  <si>
+    <t>User Defined Functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JDBC/ODBC </t>
+  </si>
+  <si>
+    <t>Caching</t>
+  </si>
+  <si>
+    <t>Output Operators</t>
+  </si>
+  <si>
+    <t>Input Sources</t>
+  </si>
+  <si>
+    <t>Transformations</t>
+  </si>
+  <si>
+    <t>Checkpointing</t>
   </si>
 </sst>
 </file>
@@ -1905,82 +1930,82 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2020,87 +2045,87 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2140,97 +2165,97 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2270,67 +2295,67 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2379,7 +2404,7 @@
     <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -2388,262 +2413,262 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="24" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
     </row>
     <row r="32" spans="2:2" ht="24" x14ac:dyDescent="0.3">
       <c r="B32" s="6" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="24" x14ac:dyDescent="0.3">
       <c r="B45" s="6" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -2653,10 +2678,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C39"/>
+  <dimension ref="B1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2828,29 +2853,29 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>96</v>
-      </c>
-    </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2863,10 +2888,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70:XFD70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2898,7 +2923,7 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2906,307 +2931,370 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>108</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>109</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>112</v>
+      <c r="B15" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>270</v>
+      <c r="B16" s="4" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>113</v>
+      <c r="B17" s="4" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>114</v>
+      <c r="B18" s="4" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>271</v>
-      </c>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>115</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>272</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>268</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>280</v>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B30" s="4" t="s">
-        <v>126</v>
+      <c r="B30" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>127</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>128</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>129</v>
+        <v>262</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>131</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>132</v>
+        <v>257</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>133</v>
+        <v>267</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>134</v>
+        <v>268</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>138</v>
+        <v>285</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>139</v>
+        <v>286</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>140</v>
+        <v>287</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
-        <v>142</v>
+        <v>288</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
-        <v>143</v>
+      <c r="B48" s="4" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>150</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B57" s="4" t="s">
-        <v>116</v>
+      <c r="B57" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>119</v>
+        <v>284</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>123</v>
+        <v>283</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B66" t="s">
-        <v>125</v>
+        <v>282</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B67" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>